<commit_message>
print out symbols that don't exist and exit
</commit_message>
<xml_diff>
--- a/TransformFidelity.xlsx
+++ b/TransformFidelity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="11475" windowHeight="8190" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="11475" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -1517,7 +1517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -1897,7 +1897,7 @@
   <dimension ref="A1:H352"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16496,7 +16496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>